<commit_message>
added homework 2 of 9A
</commit_message>
<xml_diff>
--- a/2016-07-12/FIME-5A/Homework002/db/questions.xlsx
+++ b/2016-07-12/FIME-5A/Homework002/db/questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Courses\2016-07-12\FIME-5A\Homework001\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Courses\2016-07-12\FIME-5A\Homework002\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>No</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Luis Alejandro Urbina Gonzalez</t>
+  </si>
+  <si>
+    <t>Jose Waldo Quintana Aranda</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB17"/>
+  <dimension ref="A1:BB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:M17"/>
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1222,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(2,9)</f>
@@ -1227,39 +1230,39 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:M17" ca="1" si="0">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="F2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
-      </c>
-      <c r="K2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -1275,43 +1278,43 @@
       </c>
       <c r="D3">
         <f t="shared" ref="C3:D17" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G3">
+      <c r="I3">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="H3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1323,47 +1326,47 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="D4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -1375,31 +1378,31 @@
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
@@ -1407,7 +1410,7 @@
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
@@ -1427,7 +1430,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1435,11 +1438,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
@@ -1447,23 +1450,23 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L6">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
@@ -1479,47 +1482,47 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -1531,47 +1534,47 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
@@ -1583,27 +1586,27 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
@@ -1611,7 +1614,7 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
@@ -1619,11 +1622,11 @@
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
@@ -1635,47 +1638,47 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -1687,15 +1690,15 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
@@ -1703,31 +1706,31 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="I11">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -1739,7 +1742,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
@@ -1747,39 +1750,39 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="L12">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
       <c r="M12">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -1791,47 +1794,47 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
@@ -1847,7 +1850,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
@@ -1855,35 +1858,35 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J14">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K14">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
-      </c>
-      <c r="M14">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -1903,35 +1906,35 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J15">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K15">
+      <c r="L15">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
-      </c>
-      <c r="L15">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="0"/>
@@ -1947,7 +1950,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
@@ -1955,15 +1958,15 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
@@ -1971,23 +1974,23 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1999,47 +2002,55 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="J17">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K17">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L17">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="M17">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14629184</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added questions for 5A
</commit_message>
<xml_diff>
--- a/2016-07-12/FIME-5A/Homework002/db/questions.xlsx
+++ b/2016-07-12/FIME-5A/Homework002/db/questions.xlsx
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:BB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,15 +1222,15 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:M17" ca="1" si="0">RANDBETWEEN(2,9)</f>
-        <v>4</v>
+        <f t="shared" ref="E2:O17" ca="1" si="0">RANDBETWEEN(2,9)</f>
+        <v>2</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
@@ -1238,31 +1238,91 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:X18" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>8</v>
+      </c>
+      <c r="X2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>9</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" ref="Y2:AB18" ca="1" si="2">RANDBETWEEN(2,9)</f>
+        <v>8</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -1273,20 +1333,20 @@
         <v>65</v>
       </c>
       <c r="C3">
-        <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>3</v>
+        <f t="shared" ref="C3:D17" ca="1" si="3">RANDBETWEEN(2,9)</f>
+        <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="C3:D17" ca="1" si="1">RANDBETWEEN(2,9)</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
@@ -1294,11 +1354,11 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
@@ -1306,15 +1366,75 @@
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1325,28 +1445,28 @@
         <v>55</v>
       </c>
       <c r="C4">
-        <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
@@ -1354,11 +1474,11 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
@@ -1366,6 +1486,66 @@
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -1377,48 +1557,108 @@
         <v>56</v>
       </c>
       <c r="C5">
-        <f ca="1">RANDBETWEEN(2,9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -1429,20 +1669,20 @@
         <v>66</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
@@ -1454,22 +1694,82 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -1481,16 +1781,16 @@
         <v>57</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
@@ -1498,31 +1798,91 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -1533,47 +1893,107 @@
         <v>58</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="V8">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -1585,47 +2005,107 @@
         <v>59</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="W9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" ca="1" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -1637,12 +2117,12 @@
         <v>60</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
@@ -1650,27 +2130,27 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
@@ -1678,7 +2158,67 @@
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -1689,28 +2229,28 @@
         <v>61</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
@@ -1718,19 +2258,79 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U11">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="V11">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="X11">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -1741,24 +2341,24 @@
         <v>67</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
@@ -1766,11 +2366,11 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
@@ -1778,11 +2378,71 @@
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="T12">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V12">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="W12">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="X12">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -1793,48 +2453,108 @@
         <v>62</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ref="E13:O18" ca="1" si="4">RANDBETWEEN(2,9)</f>
+        <v>8</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
       </c>
       <c r="I13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>8</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="L13">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
       <c r="M13">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="U13">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="W13">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="X13">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
@@ -1845,48 +2565,108 @@
         <v>63</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>5</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="I14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="L14">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
       </c>
       <c r="M14">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="T14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="U14">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="W14">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="X14">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -1897,48 +2677,108 @@
         <v>64</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>6</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
       <c r="I15">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
       </c>
       <c r="L15">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="M15">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="T15">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U15">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="V15">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="X15">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
@@ -1949,51 +2789,111 @@
         <v>68</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
       </c>
       <c r="I16">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="L16">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="M16">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="T16">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="X16">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14155580</v>
       </c>
@@ -2001,56 +2901,220 @@
         <v>69</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
       <c r="I17">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="J17">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="4"/>
         <v>6</v>
       </c>
       <c r="K17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
       <c r="L17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
       </c>
       <c r="M17">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="W17">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="X17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14629184</v>
       </c>
       <c r="B18" t="s">
         <v>70</v>
+      </c>
+      <c r="C18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="T18">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="V18">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="W18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>5</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>